<commit_message>
lỗi upfile danh sach sinh vien
</commit_message>
<xml_diff>
--- a/src/excelTemplate/Tao_danh_sach_lop_moi.xlsx
+++ b/src/excelTemplate/Tao_danh_sach_lop_moi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\newCDRL\src\excelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Github\newCDRL\src\excelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6E174D-2572-4C1F-BB3A-92BA6EEAE646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51682240-A818-4B7A-8148-E1E802C1E23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>MSSV</t>
   </si>
   <si>
     <t>TÊN</t>
-  </si>
-  <si>
-    <t>MẬT KHẨU</t>
   </si>
   <si>
     <t xml:space="preserve">HỌ </t>
@@ -397,20 +394,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="4" width="37.109375" customWidth="1"/>
+    <col min="2" max="3" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -418,12 +414,9 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- fix exeltemplate for create student list - Auto 0 point for students create by exel file - fix input bug can't reclick in student list of department
</commit_message>
<xml_diff>
--- a/src/excelTemplate/Tao_danh_sach_lop_moi.xlsx
+++ b/src/excelTemplate/Tao_danh_sach_lop_moi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Github\newCDRL\src\excelTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51682240-A818-4B7A-8148-E1E802C1E23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29066B9-E027-4567-9103-47B42D1FAF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,17 +30,17 @@
     <t>MSSV</t>
   </si>
   <si>
-    <t>TÊN</t>
+    <t>HỌ</t>
   </si>
   <si>
-    <t xml:space="preserve">HỌ </t>
+    <t>TÊN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +56,13 @@
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -106,12 +113,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -394,29 +404,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="2" max="3" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="1"/>
+      <c r="E1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>